<commit_message>
version 3.0 se registran datos del empleado
</commit_message>
<xml_diff>
--- a/co.com.proyectobase.screenplay/src/test/resources/datadriven/dtDatos.xlsx
+++ b/co.com.proyectobase.screenplay/src/test/resources/datadriven/dtDatos.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{ED374899-3243-4FF3-86EA-9878A49EEB81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{06AB65BD-7481-4D24-8958-C58278CD588E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12540" windowHeight="2520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14355" windowHeight="3885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>firstName</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>German Regional HQ</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Region-1</t>
+  </si>
+  <si>
+    <t>fte</t>
+  </si>
+  <si>
+    <t>temporaryDepartment</t>
+  </si>
+  <si>
+    <t>Sub unit-3</t>
+  </si>
+  <si>
+    <t>bloodGroup</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>hobbies</t>
+  </si>
+  <si>
+    <t>score goal against nacional</t>
   </si>
 </sst>
 </file>
@@ -420,7 +447,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +456,9 @@
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -455,6 +484,21 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -468,6 +512,21 @@
       </c>
       <c r="D2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>